<commit_message>
Update DateBase/orders/Fresh bloom Flowers_2025-10-15.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/Fresh bloom Flowers_2025-10-15.xlsx
+++ b/DateBase/orders/Fresh bloom Flowers_2025-10-15.xlsx
@@ -529,6 +529,9 @@
       <c r="C11" t="str">
         <v>148_坦尼克_Tineke_Rosa rugosa Thunb._20stems</v>
       </c>
+      <c r="F11" t="str">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
@@ -590,7 +593,7 @@
         <v>0.00</v>
       </c>
       <c r="G2" t="str">
-        <v>015196181942320230</v>
+        <v>0151961819423202321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>